<commit_message>
Nog wat stappen gemaakt,
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\LFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0032722B-AC53-4776-B3C8-DB1ECA44D027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBB2F86-9EC3-4BA0-93A1-97D0C7CD26AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2490" windowWidth="21840" windowHeight="13140" xr2:uid="{B2AB9483-451F-43FD-B9C9-FA638F52ACA4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Alias</t>
   </si>
@@ -233,9 +233,6 @@
     <t>QX_VENTIEL1</t>
   </si>
   <si>
-    <t>QX_VENTIEL2</t>
-  </si>
-  <si>
     <t>QX_KUKACOMMSTART</t>
   </si>
   <si>
@@ -281,12 +278,6 @@
     <t>Cuttingtool stoprelais</t>
   </si>
   <si>
-    <t>Ventiel activeer 1</t>
-  </si>
-  <si>
-    <t>Ventiel activeer 2</t>
-  </si>
-  <si>
     <t>Kuka communicatie startsignaal</t>
   </si>
   <si>
@@ -302,10 +293,106 @@
     <t>%I0.13</t>
   </si>
   <si>
-    <t>INC_TRANSBAAN</t>
-  </si>
-  <si>
-    <t>%M20</t>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>PB01</t>
+  </si>
+  <si>
+    <t>PB02</t>
+  </si>
+  <si>
+    <t>PB03</t>
+  </si>
+  <si>
+    <t>PB04</t>
+  </si>
+  <si>
+    <t>FC01</t>
+  </si>
+  <si>
+    <t>FC02</t>
+  </si>
+  <si>
+    <t>RC01</t>
+  </si>
+  <si>
+    <t>RC02</t>
+  </si>
+  <si>
+    <t>RG01</t>
+  </si>
+  <si>
+    <t>RG02</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>Y01</t>
+  </si>
+  <si>
+    <t>IKS01</t>
+  </si>
+  <si>
+    <t>IKS02</t>
+  </si>
+  <si>
+    <t>QKS01</t>
+  </si>
+  <si>
+    <t>QKS02</t>
+  </si>
+  <si>
+    <t>&lt;&lt; Kuka communicatie noodstop</t>
+  </si>
+  <si>
+    <t>Testventiel</t>
+  </si>
+  <si>
+    <t>%M98</t>
+  </si>
+  <si>
+    <t>%M99</t>
+  </si>
+  <si>
+    <t>Kuka tussengereed</t>
+  </si>
+  <si>
+    <t>IKS03</t>
+  </si>
+  <si>
+    <t>IX_KUKATUSSEN</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Kukasignaal, tussenstap voltooid</t>
+  </si>
+  <si>
+    <t>Extruder activeerknop</t>
+  </si>
+  <si>
+    <t>PB05</t>
+  </si>
+  <si>
+    <t>IX_EXTRUDERACTIEF</t>
+  </si>
+  <si>
+    <t>INGANGEN</t>
+  </si>
+  <si>
+    <t>UITGANGEN</t>
   </si>
 </sst>
 </file>
@@ -327,15 +414,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -343,12 +442,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,13 +492,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}" name="Table1" displayName="Table1" ref="C4:F28" totalsRowShown="0">
-  <autoFilter ref="C4:F28" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}" name="Table1" displayName="Table1" ref="C4:H28" totalsRowShown="0">
+  <autoFilter ref="C4:H28" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B8059A44-8B37-414C-9530-81E778E6046C}" name="Functie"/>
+    <tableColumn id="3" xr3:uid="{9EA5368B-4EBA-43F3-9D97-CD34703AB79B}" name="Label"/>
     <tableColumn id="5" xr3:uid="{C456F770-88AC-48EF-9CC1-6E0824C27C55}" name="IO Adress"/>
     <tableColumn id="2" xr3:uid="{A70383E6-EABF-4B42-8FB5-B8431F05EE1D}" name="Alias"/>
     <tableColumn id="4" xr3:uid="{2D4EFF77-16AD-4DE7-BB8B-BF9440011F39}" name="Alias memorybit"/>
+    <tableColumn id="6" xr3:uid="{DF9D7566-4D21-4B12-9F96-C5BF35619C00}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,345 +823,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65768C7D-E968-42A2-8618-9F72EE8D8ABB}">
-  <dimension ref="C4:F28"/>
+  <dimension ref="B4:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>48</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>53</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>54</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>55</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>56</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>57</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>58</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" t="s">
         <v>24</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
       <c r="C16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" t="s">
         <v>77</v>
       </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" t="s">
         <v>78</v>
       </c>
-      <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" t="s">
         <v>79</v>
       </c>
-      <c r="D21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="D22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" t="s">
         <v>80</v>
       </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
         <v>81</v>
       </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="E27" t="s">
         <v>82</v>
       </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="G27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="E28" t="s">
         <v>83</v>
       </c>
-      <c r="D25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>86</v>
+      <c r="G28" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:B18"/>
+    <mergeCell ref="B19:B28"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Config project toegevoegd, down/uploads gedaan naar fysieke PLC
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\LFT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\GitRepo\LFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBB2F86-9EC3-4BA0-93A1-97D0C7CD26AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F75B0F2-5A1D-42DA-BEE0-7D0F819CF429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="2490" windowWidth="21840" windowHeight="13140" xr2:uid="{B2AB9483-451F-43FD-B9C9-FA638F52ACA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2AB9483-451F-43FD-B9C9-FA638F52ACA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Alias</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Kuka alarmsignaal</t>
   </si>
   <si>
-    <t>Resetknop</t>
-  </si>
-  <si>
     <t>%I0.0</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>IX_STOPKNOP</t>
   </si>
   <si>
-    <t>IX_RESETKNOP</t>
-  </si>
-  <si>
     <t>IX_ESTOP</t>
   </si>
   <si>
@@ -272,12 +266,6 @@
     <t>Extruder stoprelais</t>
   </si>
   <si>
-    <t>Cuttingtool startrelais</t>
-  </si>
-  <si>
-    <t>Cuttingtool stoprelais</t>
-  </si>
-  <si>
     <t>Kuka communicatie startsignaal</t>
   </si>
   <si>
@@ -356,9 +344,6 @@
     <t>&lt;&lt; Kuka communicatie noodstop</t>
   </si>
   <si>
-    <t>Testventiel</t>
-  </si>
-  <si>
     <t>%M98</t>
   </si>
   <si>
@@ -380,26 +365,125 @@
     <t>Kukasignaal, tussenstap voltooid</t>
   </si>
   <si>
-    <t>Extruder activeerknop</t>
-  </si>
-  <si>
     <t>PB05</t>
   </si>
   <si>
-    <t>IX_EXTRUDERACTIEF</t>
-  </si>
-  <si>
     <t>INGANGEN</t>
   </si>
   <si>
     <t>UITGANGEN</t>
+  </si>
+  <si>
+    <t>Cutting toolactiveerknop</t>
+  </si>
+  <si>
+    <t>Cuttingtool start</t>
+  </si>
+  <si>
+    <t>Cuttingtool stop</t>
+  </si>
+  <si>
+    <t>Testventiel/KukaNoodstop</t>
+  </si>
+  <si>
+    <t>Klemnr.</t>
+  </si>
+  <si>
+    <t>X3-01</t>
+  </si>
+  <si>
+    <t>X3-02</t>
+  </si>
+  <si>
+    <t>X3-03</t>
+  </si>
+  <si>
+    <t>X3-04</t>
+  </si>
+  <si>
+    <t>X3-05</t>
+  </si>
+  <si>
+    <t>X3-06</t>
+  </si>
+  <si>
+    <t>X3-07</t>
+  </si>
+  <si>
+    <t>X3-08</t>
+  </si>
+  <si>
+    <t>X3-09</t>
+  </si>
+  <si>
+    <t>X3-13</t>
+  </si>
+  <si>
+    <t>X3-14</t>
+  </si>
+  <si>
+    <t>X5-K04</t>
+  </si>
+  <si>
+    <t>X6-K01</t>
+  </si>
+  <si>
+    <t>X4-06</t>
+  </si>
+  <si>
+    <t>X4-07</t>
+  </si>
+  <si>
+    <t>X4-08</t>
+  </si>
+  <si>
+    <t>X4-09</t>
+  </si>
+  <si>
+    <t>X4-10</t>
+  </si>
+  <si>
+    <t>IX_EXTRUDERHAND</t>
+  </si>
+  <si>
+    <t>24V + klem</t>
+  </si>
+  <si>
+    <t>24V - klem</t>
+  </si>
+  <si>
+    <t>X5-01</t>
+  </si>
+  <si>
+    <t>X5-02</t>
+  </si>
+  <si>
+    <t>X5-03</t>
+  </si>
+  <si>
+    <t>X5-K05</t>
+  </si>
+  <si>
+    <t>X5-K06</t>
+  </si>
+  <si>
+    <t>X5-K07</t>
+  </si>
+  <si>
+    <t>K1-24V+</t>
+  </si>
+  <si>
+    <t>K12-24V-</t>
+  </si>
+  <si>
+    <t>%M112</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +497,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,6 +522,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,15 +562,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,11 +598,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}" name="Table1" displayName="Table1" ref="C4:H28" totalsRowShown="0">
-  <autoFilter ref="C4:H28" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}" name="Table1" displayName="Table1" ref="C6:I32" totalsRowShown="0">
+  <autoFilter ref="C6:I32" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B8059A44-8B37-414C-9530-81E778E6046C}" name="Functie"/>
     <tableColumn id="3" xr3:uid="{9EA5368B-4EBA-43F3-9D97-CD34703AB79B}" name="Label"/>
+    <tableColumn id="7" xr3:uid="{0983468A-E601-4907-BC07-7A8F282E0C20}" name="Klemnr."/>
     <tableColumn id="5" xr3:uid="{C456F770-88AC-48EF-9CC1-6E0824C27C55}" name="IO Adress"/>
     <tableColumn id="2" xr3:uid="{A70383E6-EABF-4B42-8FB5-B8431F05EE1D}" name="Alias"/>
     <tableColumn id="4" xr3:uid="{2D4EFF77-16AD-4DE7-BB8B-BF9440011F39}" name="Alias memorybit"/>
@@ -823,460 +930,584 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65768C7D-E968-42A2-8618-9F72EE8D8ABB}">
-  <dimension ref="B4:H28"/>
+  <dimension ref="B6:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6"/>
+      <c r="C8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="8"/>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="8"/>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="8"/>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="8"/>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" t="s">
+        <v>146</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="8"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="7"/>
+      <c r="C24" t="s">
         <v>75</v>
       </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D24" t="s">
         <v>93</v>
       </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="7"/>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="7"/>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="7"/>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="7"/>
+      <c r="C28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" t="s">
         <v>94</v>
       </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="7"/>
+      <c r="C29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" t="s">
         <v>95</v>
       </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>101</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E29" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="7"/>
+      <c r="E30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="7"/>
+      <c r="E31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" t="s">
         <v>102</v>
       </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" t="s">
+    </row>
+    <row r="32" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="7"/>
+      <c r="E32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" t="s">
         <v>79</v>
       </c>
-      <c r="D22" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
-      <c r="H23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="H32" t="s">
         <v>103</v>
       </c>
-      <c r="E24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="E26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="E27" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" t="s">
-        <v>108</v>
-      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B5:B18"/>
-    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="B9:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Safety, Reset, andere dinkies toegevoegd
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\GitRepo\LFT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saxion-my.sharepoint.com/personal/514165_student_saxion_nl/Documents/MIA LFT handeling mechanism/06. TO (Technische Ontwerp)/PLC programma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F75B0F2-5A1D-42DA-BEE0-7D0F819CF429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{7F75B0F2-5A1D-42DA-BEE0-7D0F819CF429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2E41040-FC95-45D6-AEDD-082A45DBE781}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2AB9483-451F-43FD-B9C9-FA638F52ACA4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
   <si>
     <t>Alias</t>
   </si>
@@ -194,12 +194,6 @@
     <t>IX_FCGRIPPER</t>
   </si>
   <si>
-    <t>IX_RELAISCUTTINGOPEN</t>
-  </si>
-  <si>
-    <t>IX_RELAISCUTTINGGESLOTEN</t>
-  </si>
-  <si>
     <t>IX_REEDGRIPPER1</t>
   </si>
   <si>
@@ -477,6 +471,42 @@
   </si>
   <si>
     <t>%M112</t>
+  </si>
+  <si>
+    <t>IX_REEDCUTTINGOPEN</t>
+  </si>
+  <si>
+    <t>IX_REEDCUTTINGGESLOTEN</t>
+  </si>
+  <si>
+    <t>Klemstrook relais</t>
+  </si>
+  <si>
+    <t>X4-01</t>
+  </si>
+  <si>
+    <t>X5-K01</t>
+  </si>
+  <si>
+    <t>X4-02</t>
+  </si>
+  <si>
+    <t>X5-K02</t>
+  </si>
+  <si>
+    <t>X4-03</t>
+  </si>
+  <si>
+    <t>X5-K03</t>
+  </si>
+  <si>
+    <t>X4-04</t>
+  </si>
+  <si>
+    <t>NoodstopRelais</t>
+  </si>
+  <si>
+    <t>X4-05</t>
   </si>
 </sst>
 </file>
@@ -598,8 +628,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}" name="Table1" displayName="Table1" ref="C6:I32" totalsRowShown="0">
-  <autoFilter ref="C6:I32" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}" name="Table1" displayName="Table1" ref="C6:I37" totalsRowShown="0">
+  <autoFilter ref="C6:I37" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B8059A44-8B37-414C-9530-81E778E6046C}" name="Functie"/>
     <tableColumn id="3" xr3:uid="{9EA5368B-4EBA-43F3-9D97-CD34703AB79B}" name="Label"/>
@@ -932,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65768C7D-E968-42A2-8618-9F72EE8D8ABB}">
   <dimension ref="B6:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -953,13 +983,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -968,26 +998,26 @@
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
       <c r="C8" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -996,16 +1026,16 @@
     </row>
     <row r="9" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -1023,10 +1053,10 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -1044,10 +1074,10 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -1065,10 +1095,10 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -1086,10 +1116,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -1107,16 +1137,16 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="H14" t="s">
         <v>40</v>
@@ -1128,16 +1158,16 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="H15" t="s">
         <v>41</v>
@@ -1149,16 +1179,16 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -1170,16 +1200,16 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" t="s">
         <v>43</v>
@@ -1191,16 +1221,16 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s">
         <v>44</v>
@@ -1212,16 +1242,16 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
         <v>45</v>
@@ -1230,46 +1260,46 @@
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="8"/>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
       </c>
       <c r="G20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H20" t="s">
         <v>46</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="8"/>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -1277,13 +1307,13 @@
       <c r="B22" s="8"/>
       <c r="C22" s="3"/>
       <c r="D22" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1291,217 +1321,253 @@
     </row>
     <row r="23" spans="2:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F24" t="s">
         <v>28</v>
       </c>
       <c r="G24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
         <v>31</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
       </c>
       <c r="G28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
       </c>
       <c r="G29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
       </c>
       <c r="H30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H32" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modus functie toegevoegd. Relais uitgangen op uitgangadres, niet meer op memorybit. Geen idee waarom die het niet deden. Wat opgeschoont
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saxion-my.sharepoint.com/personal/514165_student_saxion_nl/Documents/MIA LFT handeling mechanism/06. TO (Technische Ontwerp)/PLC programma/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{7F75B0F2-5A1D-42DA-BEE0-7D0F819CF429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F94A9192-75CF-4B33-A534-CA85B11C2AE2}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{B2AB9483-451F-43FD-B9C9-FA638F52ACA4}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -209,12 +203,6 @@
     <t>QX_RELAISEXTRUDERSTOP</t>
   </si>
   <si>
-    <t>QX_RELAISCUTTINGACTIVEER</t>
-  </si>
-  <si>
-    <t>QX_RELAISCUTTINGDEACTIVEER</t>
-  </si>
-  <si>
     <t>QX_VENTIEL1</t>
   </si>
   <si>
@@ -507,13 +495,19 @@
   </si>
   <si>
     <t>X5-K3</t>
+  </si>
+  <si>
+    <t>QX_CUTTINGTOOLACTIVEER</t>
+  </si>
+  <si>
+    <t>QX_CUTTINGTOOLDEACTIVEER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,11 +522,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -592,11 +585,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -607,12 +599,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -632,16 +626,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}" name="Table1" displayName="Table1" ref="C6:I37" totalsRowShown="0">
-  <autoFilter ref="C6:I37" xr:uid="{F7B36B12-7107-4B39-8F59-06108924A04B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C6:I37" totalsRowShown="0">
+  <autoFilter ref="C6:I37"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B8059A44-8B37-414C-9530-81E778E6046C}" name="Functie"/>
-    <tableColumn id="3" xr3:uid="{9EA5368B-4EBA-43F3-9D97-CD34703AB79B}" name="Label"/>
-    <tableColumn id="7" xr3:uid="{0983468A-E601-4907-BC07-7A8F282E0C20}" name="Klemnr."/>
-    <tableColumn id="5" xr3:uid="{C456F770-88AC-48EF-9CC1-6E0824C27C55}" name="IO Adress"/>
-    <tableColumn id="2" xr3:uid="{A70383E6-EABF-4B42-8FB5-B8431F05EE1D}" name="Alias"/>
-    <tableColumn id="4" xr3:uid="{2D4EFF77-16AD-4DE7-BB8B-BF9440011F39}" name="Alias memorybit"/>
-    <tableColumn id="6" xr3:uid="{DF9D7566-4D21-4B12-9F96-C5BF35619C00}" name="Comment"/>
+    <tableColumn id="1" name="Functie"/>
+    <tableColumn id="3" name="Label"/>
+    <tableColumn id="7" name="Klemnr."/>
+    <tableColumn id="5" name="IO Adress"/>
+    <tableColumn id="2" name="Alias"/>
+    <tableColumn id="4" name="Alias memorybit"/>
+    <tableColumn id="6" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -956,44 +950,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65768C7D-E968-42A2-8618-9F72EE8D8ABB}">
-  <dimension ref="B6:I41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A6:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="162" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.08984375" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.125" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
+    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -1002,44 +996,45 @@
         <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="6"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.45" customHeight="1" thickBot="1">
+      <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="15" thickTop="1">
+      <c r="A9" s="7"/>
       <c r="B9" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1051,16 +1046,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
+      <c r="A10" s="7"/>
       <c r="B10" s="8"/>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
@@ -1072,16 +1068,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
+      <c r="A11" s="7"/>
       <c r="B11" s="8"/>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -1093,16 +1090,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
+      <c r="A12" s="7"/>
       <c r="B12" s="8"/>
-      <c r="C12" t="s">
-        <v>149</v>
+      <c r="C12" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -1114,16 +1112,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
+      <c r="A13" s="7"/>
       <c r="B13" s="8"/>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -1135,58 +1134,61 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
+      <c r="A14" s="7"/>
       <c r="B14" s="8"/>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
+      <c r="A15" s="7"/>
       <c r="B15" s="8"/>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
+      <c r="A16" s="7"/>
       <c r="B16" s="8"/>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -1198,16 +1200,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
+      <c r="A17" s="7"/>
       <c r="B17" s="8"/>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -1219,16 +1222,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
+      <c r="A18" s="7"/>
       <c r="B18" s="8"/>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
@@ -1240,16 +1244,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
+      <c r="A19" s="7"/>
       <c r="B19" s="8"/>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -1261,80 +1266,83 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
+      <c r="A20" s="7"/>
       <c r="B20" s="8"/>
-      <c r="C20" t="s">
-        <v>101</v>
+      <c r="C20" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
         <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="7"/>
       <c r="B21" s="8"/>
-      <c r="C21" t="s">
-        <v>109</v>
+      <c r="C21" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="15" thickBot="1">
+      <c r="A22" s="7"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="7" t="s">
-        <v>108</v>
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickTop="1">
+      <c r="B23" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
@@ -1343,19 +1351,19 @@
         <v>55</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="B24" s="6"/>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
@@ -1364,215 +1372,215 @@
         <v>56</v>
       </c>
       <c r="H24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="7"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="B25" s="6"/>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="7"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" s="6"/>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
       </c>
       <c r="G26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="7"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" s="6"/>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F27" t="s">
         <v>30</v>
       </c>
       <c r="G27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B28" s="7"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="B28" s="6"/>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F28" t="s">
         <v>31</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="H28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B29" s="7"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="B29" s="6"/>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F29" t="s">
         <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B30" s="7"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="B30" s="6"/>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
         <v>33</v>
       </c>
       <c r="H30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B31" s="7"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" s="6"/>
       <c r="E31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="7"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.45" customHeight="1">
+      <c r="B32" s="6"/>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="4"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="3"/>
       <c r="C33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="3"/>
+      <c r="D34" t="s">
         <v>141</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="3"/>
+      <c r="D35" t="s">
         <v>142</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" s="4"/>
-      <c r="D34" t="s">
+    <row r="36" spans="2:5">
+      <c r="B36" s="3"/>
+      <c r="D36" t="s">
         <v>143</v>
       </c>
-      <c r="E34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="4"/>
-      <c r="D35" t="s">
+      <c r="E36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="3"/>
+      <c r="C37" t="s">
         <v>144</v>
       </c>
-      <c r="E35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="4"/>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>145</v>
       </c>
-      <c r="E36" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37" s="4"/>
-      <c r="C37" t="s">
-        <v>146</v>
-      </c>
-      <c r="D37" t="s">
-        <v>147</v>
-      </c>
       <c r="E37" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B41" s="4"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Wat een kutaddressen allemaal. Moet een aantal bits voorbereiden voor schrijven naar uitgangen
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -212,15 +212,6 @@
     <t>QX_KUKACOMMSTOP</t>
   </si>
   <si>
-    <t>%M90</t>
-  </si>
-  <si>
-    <t>%M91</t>
-  </si>
-  <si>
-    <t>%M92</t>
-  </si>
-  <si>
     <t>%M93</t>
   </si>
   <si>
@@ -501,6 +492,15 @@
   </si>
   <si>
     <t>QX_CUTTINGTOOLDEACTIVEER</t>
+  </si>
+  <si>
+    <t>%M60-%M62</t>
+  </si>
+  <si>
+    <t>%M81</t>
+  </si>
+  <si>
+    <t>%M80</t>
   </si>
 </sst>
 </file>
@@ -596,14 +596,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,7 +950,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -961,7 +961,7 @@
   <dimension ref="A6:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -981,13 +981,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -996,26 +996,26 @@
         <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.45" customHeight="1" thickBot="1">
       <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1023,18 +1023,18 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="15" thickTop="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1047,16 +1047,16 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
@@ -1069,16 +1069,16 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -1091,16 +1091,16 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7" t="s">
-        <v>147</v>
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -1113,16 +1113,16 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="7" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -1135,60 +1135,60 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="7" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="7" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="7" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -1201,16 +1201,16 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="7" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -1223,16 +1223,16 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="7" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
@@ -1245,16 +1245,16 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="7" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -1267,82 +1267,82 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="7" t="s">
-        <v>99</v>
+      <c r="A20" s="6"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F20" t="s">
         <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="7" t="s">
-        <v>107</v>
+      <c r="A21" s="6"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" thickTop="1">
-      <c r="B23" s="6" t="s">
-        <v>106</v>
+      <c r="B23" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
@@ -1351,19 +1351,19 @@
         <v>55</v>
       </c>
       <c r="H23" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="B24" s="6"/>
+      <c r="B24" s="8"/>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
@@ -1372,19 +1372,19 @@
         <v>56</v>
       </c>
       <c r="H24" t="s">
-        <v>61</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="B25" s="6"/>
+      <c r="B25" s="8"/>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
@@ -1393,19 +1393,19 @@
         <v>58</v>
       </c>
       <c r="H25" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="B26" s="6"/>
+      <c r="B26" s="8"/>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
@@ -1414,19 +1414,19 @@
         <v>59</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="B27" s="6"/>
+      <c r="B27" s="8"/>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
         <v>30</v>
@@ -1435,139 +1435,139 @@
         <v>57</v>
       </c>
       <c r="H27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="B28" s="6"/>
+      <c r="B28" s="8"/>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F28" t="s">
         <v>31</v>
       </c>
       <c r="G28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="B29" s="6"/>
+      <c r="B29" s="8"/>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F29" t="s">
         <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="B30" s="6"/>
+      <c r="B30" s="8"/>
       <c r="E30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F30" t="s">
         <v>33</v>
       </c>
       <c r="H30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="B31" s="6"/>
+      <c r="B31" s="8"/>
       <c r="E31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.45" customHeight="1">
-      <c r="B32" s="6"/>
+      <c r="B32" s="8"/>
       <c r="E32" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="3"/>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E33" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="3"/>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E34" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="3"/>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E35" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="3"/>
       <c r="D36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="3"/>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="2:5">

</xml_diff>

<commit_message>
Merkertest gedaan. Dut't nie
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="157">
   <si>
     <t>Alias</t>
   </si>
@@ -107,9 +107,6 @@
     <t>%I0.12</t>
   </si>
   <si>
-    <t>Alias memorybit</t>
-  </si>
-  <si>
     <t>%Q0.0</t>
   </si>
   <si>
@@ -212,21 +209,6 @@
     <t>QX_KUKACOMMSTOP</t>
   </si>
   <si>
-    <t>%M93</t>
-  </si>
-  <si>
-    <t>%M94</t>
-  </si>
-  <si>
-    <t>%M95</t>
-  </si>
-  <si>
-    <t>%M96</t>
-  </si>
-  <si>
-    <t>%M97</t>
-  </si>
-  <si>
     <t>IO Adress</t>
   </si>
   <si>
@@ -497,10 +479,28 @@
     <t>%M60-%M62</t>
   </si>
   <si>
-    <t>%M81</t>
-  </si>
-  <si>
-    <t>%M80</t>
+    <t>Alias memorybits</t>
+  </si>
+  <si>
+    <t>%M65-%M67</t>
+  </si>
+  <si>
+    <t>%M68-%M70</t>
+  </si>
+  <si>
+    <t>%M71-%M73</t>
+  </si>
+  <si>
+    <t>%M74-%M76</t>
+  </si>
+  <si>
+    <t>%M77-%M79</t>
+  </si>
+  <si>
+    <t>%M80-%M83</t>
+  </si>
+  <si>
+    <t>&lt; transportbaan reserve</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
     <tableColumn id="7" name="Klemnr."/>
     <tableColumn id="5" name="IO Adress"/>
     <tableColumn id="2" name="Alias"/>
-    <tableColumn id="4" name="Alias memorybit"/>
+    <tableColumn id="4" name="Alias memorybits"/>
     <tableColumn id="6" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -950,7 +950,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -971,8 +971,8 @@
     <col min="4" max="4" width="8.125" customWidth="1"/>
     <col min="5" max="5" width="11.875" customWidth="1"/>
     <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -981,41 +981,41 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.45" customHeight="1" thickBot="1">
       <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1025,25 +1025,25 @@
     <row r="9" spans="1:9" ht="15" thickTop="1">
       <c r="A9" s="6"/>
       <c r="B9" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1053,19 +1053,19 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1075,41 +1075,41 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="6"/>
       <c r="B12" s="9"/>
       <c r="C12" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1119,19 +1119,19 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1141,19 +1141,19 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1163,19 +1163,19 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1185,19 +1185,19 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1207,19 +1207,19 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1229,19 +1229,19 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1251,66 +1251,66 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6"/>
       <c r="B20" s="9"/>
       <c r="C20" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F20" t="s">
         <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -1319,13 +1319,13 @@
       <c r="B22" s="9"/>
       <c r="C22" s="7"/>
       <c r="D22" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1333,241 +1333,244 @@
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" thickTop="1">
       <c r="B23" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="B24" s="8"/>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="B25" s="8"/>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H25" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="B26" s="8"/>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="B27" s="8"/>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H27" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="I27" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="B28" s="8"/>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H28" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="B29" s="8"/>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G29" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H29" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="B30" s="8"/>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="B31" s="8"/>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H31" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="I31" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.45" customHeight="1">
       <c r="B32" s="8"/>
       <c r="E32" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H32" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="I32" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="3"/>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="3"/>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E34" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="3"/>
       <c r="D35" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E35" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="3"/>
       <c r="D36" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E36" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="3"/>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E37" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="2:5">

</xml_diff>

<commit_message>
Alias vernieuwd. PRG loopt. Weg ermee
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -950,7 +950,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
testje gedaan op de testopstelling
</commit_message>
<xml_diff>
--- a/IOlijst.xlsx
+++ b/IOlijst.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saxion-my.sharepoint.com/personal/514165_student_saxion_nl/Documents/MIA LFT handeling mechanism/06. TO (Technische Ontwerp)/Besturing/PLC/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_F054B06C10BB6C603BEFA78A616EECCE8489E478" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A368F1AD-C3AC-4F54-97E7-ECD8F09752CD}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="158">
   <si>
     <t>Alias</t>
   </si>
@@ -501,13 +496,16 @@
   </si>
   <si>
     <t>&lt; transportbaan reserve</t>
+  </si>
+  <si>
+    <t>Reset ding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,21 +619,17 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C6:I37" totalsRowShown="0">
-  <autoFilter ref="C6:I37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="C6:I37" totalsRowShown="0">
+  <autoFilter ref="C6:I37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Functie"/>
-    <tableColumn id="3" name="Label"/>
-    <tableColumn id="7" name="Klemnr."/>
-    <tableColumn id="5" name="IO Adress"/>
-    <tableColumn id="2" name="Alias"/>
-    <tableColumn id="4" name="Alias memorybits"/>
-    <tableColumn id="6" name="Comment"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Functie"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Label"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Klemnr."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IO Adress"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Alias"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Alias memorybits"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -950,33 +944,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:I41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A6:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="29.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -999,7 +993,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>121</v>
@@ -1008,7 +1002,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" customHeight="1" thickBot="1">
+    <row r="8" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
         <v>122</v>
@@ -1022,7 +1016,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="15" thickTop="1">
+    <row r="9" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="9" t="s">
         <v>96</v>
@@ -1046,7 +1040,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="9"/>
       <c r="C10" s="6" t="s">
@@ -1068,7 +1062,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="9"/>
       <c r="C11" s="6" t="s">
@@ -1090,7 +1084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="9"/>
       <c r="C12" s="6" t="s">
@@ -1112,7 +1106,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="9"/>
       <c r="C13" s="6" t="s">
@@ -1134,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="9"/>
       <c r="C14" s="6" t="s">
@@ -1156,7 +1150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="9"/>
       <c r="C15" s="6" t="s">
@@ -1178,7 +1172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="9"/>
       <c r="C16" s="6" t="s">
@@ -1200,7 +1194,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="9"/>
       <c r="C17" s="6" t="s">
@@ -1222,7 +1216,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="9"/>
       <c r="C18" s="6" t="s">
@@ -1244,7 +1238,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="9"/>
       <c r="C19" s="6" t="s">
@@ -1266,7 +1260,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="9"/>
       <c r="C20" s="6" t="s">
@@ -1291,7 +1285,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6" t="s">
@@ -1314,7 +1308,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="9"/>
       <c r="C22" s="7"/>
@@ -1331,7 +1325,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" thickTop="1">
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>97</v>
       </c>
@@ -1354,7 +1348,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
       <c r="C24" t="s">
         <v>61</v>
@@ -1375,7 +1369,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" s="8"/>
       <c r="C25" t="s">
         <v>62</v>
@@ -1396,7 +1390,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
       <c r="C26" t="s">
         <v>63</v>
@@ -1417,7 +1411,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
       <c r="C27" t="s">
         <v>101</v>
@@ -1441,7 +1435,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="8"/>
       <c r="C28" t="s">
         <v>99</v>
@@ -1462,7 +1456,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29" s="8"/>
       <c r="C29" t="s">
         <v>100</v>
@@ -1483,7 +1477,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
       <c r="E30" t="s">
         <v>117</v>
@@ -1492,7 +1486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
       <c r="E31" t="s">
         <v>118</v>
@@ -1507,7 +1501,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14.45" customHeight="1">
+    <row r="32" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
       <c r="E32" t="s">
         <v>119</v>
@@ -1522,7 +1516,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="3"/>
       <c r="C33" t="s">
         <v>130</v>
@@ -1534,7 +1528,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="3"/>
       <c r="D34" t="s">
         <v>132</v>
@@ -1543,7 +1537,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="3"/>
       <c r="D35" t="s">
         <v>133</v>
@@ -1552,7 +1546,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="D36" t="s">
         <v>134</v>
@@ -1561,7 +1555,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="3"/>
       <c r="C37" t="s">
         <v>135</v>
@@ -1573,17 +1567,22 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="3"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>